<commit_message>
Updated the affixes pages, fixed a couple bugs.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Affixes/entrancing.xlsx
+++ b/resources/data-imports/Affixes/entrancing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="89">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t xml:space="preserve">resistance_reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">affix_type</t>
   </si>
   <si>
     <t xml:space="preserve">Magicians Trance</t>
@@ -389,10 +392,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM25"/>
+  <dimension ref="A1:AN25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI2" activeCellId="0" sqref="AI2:AI25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AN2" activeCellId="0" sqref="AN2:AN25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -545,16 +548,19 @@
       <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="AN1" s="0" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L2" s="1" t="n">
         <v>0</v>
@@ -605,7 +611,7 @@
         <v>1000</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ2" s="1" t="n">
         <v>0.01</v>
@@ -618,6 +624,9 @@
       </c>
       <c r="AM2" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN2" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,10 +634,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L3" s="1" t="n">
         <v>0</v>
@@ -679,7 +688,7 @@
         <v>2141</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ3" s="1" t="n">
         <v>0.0122</v>
@@ -692,6 +701,9 @@
       </c>
       <c r="AM3" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN3" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -699,10 +711,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L4" s="1" t="n">
         <v>0</v>
@@ -753,7 +765,7 @@
         <v>4582</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ4" s="1" t="n">
         <v>0.0149</v>
@@ -766,6 +778,9 @@
       </c>
       <c r="AM4" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN4" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,10 +788,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L5" s="1" t="n">
         <v>0</v>
@@ -827,7 +842,7 @@
         <v>9808</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ5" s="1" t="n">
         <v>0.0182</v>
@@ -840,6 +855,9 @@
       </c>
       <c r="AM5" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN5" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -847,10 +865,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L6" s="1" t="n">
         <v>0</v>
@@ -901,7 +919,7 @@
         <v>21000</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ6" s="1" t="n">
         <v>0.0223</v>
@@ -914,6 +932,9 @@
       </c>
       <c r="AM6" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN6" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -921,10 +942,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L7" s="1" t="n">
         <v>0</v>
@@ -975,7 +996,7 @@
         <v>44900</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ7" s="1" t="n">
         <v>0.0272</v>
@@ -988,6 +1009,9 @@
       </c>
       <c r="AM7" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN7" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,10 +1019,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L8" s="1" t="n">
         <v>0</v>
@@ -1049,7 +1073,7 @@
         <v>96200</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ8" s="1" t="n">
         <v>0.0332</v>
@@ -1062,6 +1086,9 @@
       </c>
       <c r="AM8" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN8" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1069,10 +1096,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L9" s="1" t="n">
         <v>0</v>
@@ -1123,7 +1150,7 @@
         <v>205900</v>
       </c>
       <c r="AI9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ9" s="1" t="n">
         <v>0.0406</v>
@@ -1136,6 +1163,9 @@
       </c>
       <c r="AM9" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN9" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,10 +1173,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L10" s="1" t="n">
         <v>0</v>
@@ -1197,7 +1227,7 @@
         <v>440800</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ10" s="1" t="n">
         <v>0.0496</v>
@@ -1210,6 +1240,9 @@
       </c>
       <c r="AM10" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN10" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1217,10 +1250,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L11" s="1" t="n">
         <v>0</v>
@@ -1271,7 +1304,7 @@
         <v>943500</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ11" s="1" t="n">
         <v>0.0606</v>
@@ -1284,6 +1317,9 @@
       </c>
       <c r="AM11" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN11" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,10 +1327,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L12" s="1" t="n">
         <v>0</v>
@@ -1345,7 +1381,7 @@
         <v>2019500</v>
       </c>
       <c r="AI12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ12" s="1" t="n">
         <v>0.0741</v>
@@ -1358,6 +1394,9 @@
       </c>
       <c r="AM12" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN12" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1365,10 +1404,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L13" s="1" t="n">
         <v>0</v>
@@ -1419,7 +1458,7 @@
         <v>4322800</v>
       </c>
       <c r="AI13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ13" s="1" t="n">
         <v>0.0905</v>
@@ -1432,6 +1471,9 @@
       </c>
       <c r="AM13" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN13" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1439,10 +1481,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L14" s="1" t="n">
         <v>0</v>
@@ -1493,7 +1535,7 @@
         <v>10451500</v>
       </c>
       <c r="AI14" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ14" s="1" t="n">
         <v>0.1248</v>
@@ -1506,6 +1548,9 @@
       </c>
       <c r="AM14" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN14" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1513,10 +1558,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L15" s="1" t="n">
         <v>0</v>
@@ -1567,7 +1612,7 @@
         <v>22600200</v>
       </c>
       <c r="AI15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ15" s="1" t="n">
         <v>0.1541</v>
@@ -1580,6 +1625,9 @@
       </c>
       <c r="AM15" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN15" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,10 +1635,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L16" s="1" t="n">
         <v>0</v>
@@ -1641,7 +1689,7 @@
         <v>48870200</v>
       </c>
       <c r="AI16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ16" s="1" t="n">
         <v>0.1901</v>
@@ -1654,6 +1702,9 @@
       </c>
       <c r="AM16" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN16" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1661,10 +1712,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L17" s="1" t="n">
         <v>0</v>
@@ -1715,7 +1766,7 @@
         <v>105675800</v>
       </c>
       <c r="AI17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ17" s="1" t="n">
         <v>0.2347</v>
@@ -1728,6 +1779,9 @@
       </c>
       <c r="AM17" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN17" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1735,10 +1789,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L18" s="1" t="n">
         <v>0</v>
@@ -1789,7 +1843,7 @@
         <v>228511100</v>
       </c>
       <c r="AI18" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ18" s="1" t="n">
         <v>0.2896</v>
@@ -1802,6 +1856,9 @@
       </c>
       <c r="AM18" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN18" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1809,10 +1866,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L19" s="1" t="n">
         <v>0</v>
@@ -1863,7 +1920,7 @@
         <v>494127600</v>
       </c>
       <c r="AI19" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ19" s="1" t="n">
         <v>0.3574</v>
@@ -1876,6 +1933,9 @@
       </c>
       <c r="AM19" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN19" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1883,10 +1943,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L20" s="1" t="n">
         <v>0</v>
@@ -1937,7 +1997,7 @@
         <v>1068490900</v>
       </c>
       <c r="AI20" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ20" s="1" t="n">
         <v>0.4411</v>
@@ -1950,6 +2010,9 @@
       </c>
       <c r="AM20" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN20" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1957,10 +2020,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L21" s="1" t="n">
         <v>0</v>
@@ -2011,7 +2074,7 @@
         <v>2310481600</v>
       </c>
       <c r="AI21" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ21" s="1" t="n">
         <v>0.5444</v>
@@ -2024,6 +2087,9 @@
       </c>
       <c r="AM21" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN21" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2031,10 +2097,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L22" s="1" t="n">
         <v>0</v>
@@ -2085,7 +2151,7 @@
         <v>4996135800</v>
       </c>
       <c r="AI22" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ22" s="1" t="n">
         <v>0.6719</v>
@@ -2098,6 +2164,9 @@
       </c>
       <c r="AM22" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN22" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2105,10 +2174,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L23" s="1" t="n">
         <v>0</v>
@@ -2159,7 +2228,7 @@
         <v>10803536500</v>
       </c>
       <c r="AI23" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ23" s="1" t="n">
         <v>0.802</v>
@@ -2172,6 +2241,9 @@
       </c>
       <c r="AM23" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN23" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2179,10 +2251,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L24" s="1" t="n">
         <v>0</v>
@@ -2233,7 +2305,7 @@
         <v>23361334900</v>
       </c>
       <c r="AI24" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ24" s="1" t="n">
         <v>0.804</v>
@@ -2246,6 +2318,9 @@
       </c>
       <c r="AM24" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN24" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,10 +2328,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L25" s="1" t="n">
         <v>0</v>
@@ -2307,7 +2382,7 @@
         <v>40000000000</v>
       </c>
       <c r="AI25" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ25" s="1" t="n">
         <v>1</v>
@@ -2320,6 +2395,9 @@
       </c>
       <c r="AM25" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="AN25" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>